<commit_message>
Fixed typos and expanded description of the simulations and results, corrected file names
</commit_message>
<xml_diff>
--- a/Summary data final.xlsx
+++ b/Summary data final.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwnetid-my.sharepoint.com/personal/dtlinker_uw_edu/Documents/CFD Tool stenosis/For article/Prosthetic-AoV-CFD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B2A24802-29E4-B844-882C-E1521ABB5A73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{B2A24802-29E4-B844-882C-E1521ABB5A73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A082D61E-38F5-314A-82D5-4ECA292D46D1}"/>
   <bookViews>
     <workbookView xWindow="5460" yWindow="1300" windowWidth="20980" windowHeight="17040" xr2:uid="{9C2AD0E6-F596-254D-B62A-EC708624402D}"/>
   </bookViews>
@@ -482,7 +482,7 @@
   <dimension ref="A1:O64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:O64"/>
+      <selection sqref="A1:O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -491,7 +491,8 @@
     <col min="2" max="2" width="5.83203125" customWidth="1"/>
     <col min="3" max="3" width="4.6640625" customWidth="1"/>
     <col min="4" max="4" width="6.6640625" customWidth="1"/>
-    <col min="5" max="6" width="4.5" customWidth="1"/>
+    <col min="5" max="5" width="4.5" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" customWidth="1"/>
     <col min="7" max="7" width="6.1640625" customWidth="1"/>
     <col min="8" max="8" width="5" customWidth="1"/>
     <col min="9" max="9" width="7.5" customWidth="1"/>
@@ -2263,7 +2264,7 @@
         <v>7</v>
       </c>
       <c r="F34" s="1">
-        <f t="shared" ref="F34:F65" si="6">PI()*(E34/10)^2</f>
+        <f t="shared" ref="F34:F64" si="6">PI()*(E34/10)^2</f>
         <v>1.5393804002589984</v>
       </c>
       <c r="G34" s="1">
@@ -3896,6 +3897,7 @@
     <sortCondition descending="1" ref="A2:A64"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>